<commit_message>
finished size up room analysis
</commit_message>
<xml_diff>
--- a/brynmawr/fallAnalysis.xlsx
+++ b/brynmawr/fallAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dndin\Documents\CS340\project\cs340-project\brynmawr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33856FC-2C3A-4F9B-BCAD-9C78503626C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8234D55D-CC5C-40D6-8F6D-03BB7197EF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2820" windowWidth="14280" windowHeight="10410" activeTab="1" xr2:uid="{41F0CD19-36E9-4CA9-A6FE-2857FFC324B3}"/>
+    <workbookView xWindow="11700" yWindow="3435" windowWidth="14280" windowHeight="10410" activeTab="2" xr2:uid="{41F0CD19-36E9-4CA9-A6FE-2857FFC324B3}"/>
   </bookViews>
   <sheets>
     <sheet name="no constraints" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
   <si>
     <t>Classes</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>This does not have room constraints either</t>
-  </si>
-  <si>
-    <t>0.008996963500976562 seconds</t>
   </si>
   <si>
     <t>Diff Exp</t>
@@ -977,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E44F4F0E-97F0-448B-85BF-165CA56B88B0}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
@@ -1021,10 +1018,10 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1651,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFABE1D-3621-4D95-B00E-DC62BD93ED73}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,10 +1691,10 @@
         <v>7</v>
       </c>
       <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1720,7 +1717,7 @@
         <v>60</v>
       </c>
       <c r="G2">
-        <v>4.0020942687988203E-3</v>
+        <v>1.30233764648437E-2</v>
       </c>
       <c r="H2">
         <v>3497</v>
@@ -1761,25 +1758,25 @@
         <v>59</v>
       </c>
       <c r="G3">
-        <v>9.9999904632568307E-3</v>
+        <v>1.0282039642333899E-2</v>
       </c>
       <c r="H3">
         <v>3542</v>
       </c>
       <c r="I3">
-        <v>3174</v>
+        <v>3173</v>
       </c>
       <c r="J3">
         <f t="shared" ref="J3:J16" si="0">I3/H3</f>
-        <v>0.89610389610389607</v>
+        <v>0.89582156973461324</v>
       </c>
       <c r="K3">
         <f>I3-'no constraints'!I3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <f>J3-'no constraints'!J3</f>
-        <v>2.8232636928282595E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1802,7 +1799,7 @@
         <v>61</v>
       </c>
       <c r="G4">
-        <v>3.9999485015869097E-3</v>
+        <v>1.0424852371215799E-2</v>
       </c>
       <c r="H4">
         <v>3579</v>
@@ -1843,25 +1840,25 @@
         <v>59</v>
       </c>
       <c r="G5">
-        <v>4.0020942687988203E-3</v>
+        <v>1.31230354309082E-2</v>
       </c>
       <c r="H5">
         <v>3539</v>
       </c>
       <c r="I5">
-        <v>3159</v>
+        <v>3161</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0.89262503532071202</v>
+        <v>0.89319016671376095</v>
       </c>
       <c r="K5">
         <f>I5-'no constraints'!I5</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L5">
         <f>J5-'no constraints'!J5</f>
-        <v>1.9779598756710648E-3</v>
+        <v>2.543091268719988E-3</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1883,8 +1880,8 @@
       <c r="F6">
         <v>51</v>
       </c>
-      <c r="G6" t="s">
-        <v>11</v>
+      <c r="G6">
+        <v>9.8819732666015608E-3</v>
       </c>
       <c r="H6">
         <v>3700</v>
@@ -1925,7 +1922,7 @@
         <v>52</v>
       </c>
       <c r="G7">
-        <v>8.9969635009765608E-3</v>
+        <v>1.1027812957763601E-2</v>
       </c>
       <c r="H7">
         <v>3680</v>
@@ -1966,7 +1963,7 @@
         <v>63</v>
       </c>
       <c r="G8">
-        <v>4.9865245819091797E-3</v>
+        <v>1.2421846389770499E-2</v>
       </c>
       <c r="H8">
         <v>3798</v>
@@ -2007,7 +2004,7 @@
         <v>62</v>
       </c>
       <c r="G9">
-        <v>7.9994201660156198E-3</v>
+        <v>1.1552095413207999E-2</v>
       </c>
       <c r="H9">
         <v>3862</v>
@@ -2048,7 +2045,7 @@
         <v>63</v>
       </c>
       <c r="G10">
-        <v>8.0056190490722604E-3</v>
+        <v>1.26750469207763E-2</v>
       </c>
       <c r="H10">
         <v>3794</v>
@@ -2089,7 +2086,7 @@
         <v>67</v>
       </c>
       <c r="G11">
-        <v>3.9997100830078099E-3</v>
+        <v>1.07879638671875E-2</v>
       </c>
       <c r="H11">
         <v>4057</v>
@@ -2130,7 +2127,7 @@
         <v>68</v>
       </c>
       <c r="G12">
-        <v>7.9998970031738195E-3</v>
+        <v>1.60486698150634E-2</v>
       </c>
       <c r="H12">
         <v>4466</v>
@@ -2171,7 +2168,7 @@
         <v>64</v>
       </c>
       <c r="G13">
-        <v>7.9998970031738195E-3</v>
+        <v>1.2868881225585899E-2</v>
       </c>
       <c r="H13">
         <v>4671</v>
@@ -2212,7 +2209,7 @@
         <v>70</v>
       </c>
       <c r="G14">
-        <v>4.0059089660644497E-3</v>
+        <v>1.2700080871582E-2</v>
       </c>
       <c r="H14">
         <v>4813</v>
@@ -2253,7 +2250,7 @@
         <v>69</v>
       </c>
       <c r="G15">
-        <v>3.953218460083E-3</v>
+        <v>1.6459941864013599E-2</v>
       </c>
       <c r="H15">
         <v>4739</v>
@@ -2294,25 +2291,25 @@
         <v>67</v>
       </c>
       <c r="G16">
-        <v>8.0018043518066406E-3</v>
+        <v>1.4331102371215799E-2</v>
       </c>
       <c r="H16">
         <v>4558</v>
       </c>
       <c r="I16">
-        <v>4173</v>
+        <v>4169</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0.91553312856516011</v>
+        <v>0.91465555068012283</v>
       </c>
       <c r="K16">
         <f>I16-'no constraints'!I16</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L16">
         <f>J16-'no constraints'!J16</f>
-        <v>1.7551557700745679E-3</v>
+        <v>8.7757788503728396E-4</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -2322,5 +2319,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added data for subject constraint
</commit_message>
<xml_diff>
--- a/brynmawr/fallAnalysis.xlsx
+++ b/brynmawr/fallAnalysis.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dndin\Documents\CS340\project\cs340-project\brynmawr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8234D55D-CC5C-40D6-8F6D-03BB7197EF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88F9FBB-98BC-4100-ADED-DB84D8C1972B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="3435" windowWidth="14280" windowHeight="10410" activeTab="2" xr2:uid="{41F0CD19-36E9-4CA9-A6FE-2857FFC324B3}"/>
+    <workbookView xWindow="3840" yWindow="2475" windowWidth="14280" windowHeight="10410" firstSheet="2" activeTab="3" xr2:uid="{41F0CD19-36E9-4CA9-A6FE-2857FFC324B3}"/>
   </bookViews>
   <sheets>
     <sheet name="no constraints" sheetId="1" r:id="rId1"/>
     <sheet name="room constraint" sheetId="2" r:id="rId2"/>
     <sheet name="increasing room size" sheetId="3" r:id="rId3"/>
+    <sheet name="limiting subject conflict" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="13">
   <si>
     <t>Classes</t>
   </si>
@@ -1648,8 +1649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFABE1D-3621-4D95-B00E-DC62BD93ED73}">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,4 +2322,672 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52293D6E-ACFD-4E22-982B-246A4AD891D0}">
+  <dimension ref="A1:L16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2000</v>
+      </c>
+      <c r="B2">
+        <v>231</v>
+      </c>
+      <c r="C2">
+        <v>164</v>
+      </c>
+      <c r="D2">
+        <v>1112</v>
+      </c>
+      <c r="E2">
+        <v>17</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <v>7.9793930053710903E-3</v>
+      </c>
+      <c r="H2">
+        <v>3497</v>
+      </c>
+      <c r="I2">
+        <v>3133</v>
+      </c>
+      <c r="J2">
+        <f>I2/H2</f>
+        <v>0.89591078066914498</v>
+      </c>
+      <c r="K2">
+        <f>I2-'no constraints'!I2</f>
+        <v>5</v>
+      </c>
+      <c r="L2">
+        <f>J2-'no constraints'!J2</f>
+        <v>1.429796968830388E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2001</v>
+      </c>
+      <c r="B3">
+        <v>222</v>
+      </c>
+      <c r="C3">
+        <v>167</v>
+      </c>
+      <c r="D3">
+        <v>1096</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>59</v>
+      </c>
+      <c r="G3">
+        <v>4.9862861633300703E-3</v>
+      </c>
+      <c r="H3">
+        <v>3542</v>
+      </c>
+      <c r="I3">
+        <v>3189</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J16" si="0">I3/H3</f>
+        <v>0.90033879164313946</v>
+      </c>
+      <c r="K3">
+        <f>I3-'no constraints'!I3</f>
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <f>J3-'no constraints'!J3</f>
+        <v>4.5172219085262144E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2002</v>
+      </c>
+      <c r="B4">
+        <v>239</v>
+      </c>
+      <c r="C4">
+        <v>159</v>
+      </c>
+      <c r="D4">
+        <v>1090</v>
+      </c>
+      <c r="E4">
+        <v>17</v>
+      </c>
+      <c r="F4">
+        <v>61</v>
+      </c>
+      <c r="G4">
+        <v>4.0507316589355399E-3</v>
+      </c>
+      <c r="H4">
+        <v>3579</v>
+      </c>
+      <c r="I4">
+        <v>3112</v>
+      </c>
+      <c r="J4">
+        <f>I4/H4</f>
+        <v>0.86951662475551827</v>
+      </c>
+      <c r="K4">
+        <f>I4-'no constraints'!I4</f>
+        <v>-3</v>
+      </c>
+      <c r="L4">
+        <f>J4-'no constraints'!J4</f>
+        <v>-8.382229673092878E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2003</v>
+      </c>
+      <c r="B5">
+        <v>241</v>
+      </c>
+      <c r="C5">
+        <v>151</v>
+      </c>
+      <c r="D5">
+        <v>1104</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5">
+        <v>59</v>
+      </c>
+      <c r="G5">
+        <v>8.0018043518066406E-3</v>
+      </c>
+      <c r="H5">
+        <v>3539</v>
+      </c>
+      <c r="I5">
+        <v>3168</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.89516812658943201</v>
+      </c>
+      <c r="K5">
+        <f>I5-'no constraints'!I5</f>
+        <v>16</v>
+      </c>
+      <c r="L5">
+        <f>J5-'no constraints'!J5</f>
+        <v>4.5210511443910528E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2004</v>
+      </c>
+      <c r="B6">
+        <v>265</v>
+      </c>
+      <c r="C6">
+        <v>163</v>
+      </c>
+      <c r="D6">
+        <v>1124</v>
+      </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>51</v>
+      </c>
+      <c r="G6">
+        <v>4.9865245819091797E-3</v>
+      </c>
+      <c r="H6">
+        <v>3700</v>
+      </c>
+      <c r="I6">
+        <v>3339</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.90243243243243243</v>
+      </c>
+      <c r="K6">
+        <f>I6-'no constraints'!I6</f>
+        <v>31</v>
+      </c>
+      <c r="L6">
+        <f>J6-'no constraints'!J6</f>
+        <v>8.3783783783784038E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2005</v>
+      </c>
+      <c r="B7">
+        <v>255</v>
+      </c>
+      <c r="C7">
+        <v>156</v>
+      </c>
+      <c r="D7">
+        <v>1127</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>52</v>
+      </c>
+      <c r="G7">
+        <v>6.0017108917236302E-3</v>
+      </c>
+      <c r="H7">
+        <v>3680</v>
+      </c>
+      <c r="I7">
+        <v>3304</v>
+      </c>
+      <c r="J7">
+        <f>I7/H7</f>
+        <v>0.89782608695652177</v>
+      </c>
+      <c r="K7">
+        <f>I7-'no constraints'!I7</f>
+        <v>38</v>
+      </c>
+      <c r="L7">
+        <f>J7-'no constraints'!J7</f>
+        <v>1.0326086956521818E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2006</v>
+      </c>
+      <c r="B8">
+        <v>269</v>
+      </c>
+      <c r="C8">
+        <v>169</v>
+      </c>
+      <c r="D8">
+        <v>1167</v>
+      </c>
+      <c r="E8">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>63</v>
+      </c>
+      <c r="G8">
+        <v>8.0003738403320295E-3</v>
+      </c>
+      <c r="H8">
+        <v>3798</v>
+      </c>
+      <c r="I8">
+        <v>3391</v>
+      </c>
+      <c r="J8">
+        <f>I8/H8</f>
+        <v>0.89283833596629802</v>
+      </c>
+      <c r="K8">
+        <f>I8-'no constraints'!I8</f>
+        <v>12</v>
+      </c>
+      <c r="L8">
+        <f>J8-'no constraints'!J8</f>
+        <v>3.1595576619273258E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2007</v>
+      </c>
+      <c r="B9">
+        <v>283</v>
+      </c>
+      <c r="C9">
+        <v>169</v>
+      </c>
+      <c r="D9">
+        <v>1148</v>
+      </c>
+      <c r="E9">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>62</v>
+      </c>
+      <c r="G9">
+        <v>6.9813728332519497E-3</v>
+      </c>
+      <c r="H9">
+        <v>3862</v>
+      </c>
+      <c r="I9">
+        <v>3480</v>
+      </c>
+      <c r="J9">
+        <f>I9/H9</f>
+        <v>0.90108751941998966</v>
+      </c>
+      <c r="K9">
+        <f>I9-'no constraints'!I9</f>
+        <v>31</v>
+      </c>
+      <c r="L9">
+        <f>J9-'no constraints'!J9</f>
+        <v>8.02692905230451E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2008</v>
+      </c>
+      <c r="B10">
+        <v>284</v>
+      </c>
+      <c r="C10">
+        <v>175</v>
+      </c>
+      <c r="D10">
+        <v>1213</v>
+      </c>
+      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>63</v>
+      </c>
+      <c r="G10">
+        <v>7.9994201660156198E-3</v>
+      </c>
+      <c r="H10">
+        <v>3794</v>
+      </c>
+      <c r="I10">
+        <v>3410</v>
+      </c>
+      <c r="J10">
+        <f>I10/H10</f>
+        <v>0.89878755930416443</v>
+      </c>
+      <c r="K10">
+        <f>I10-'no constraints'!I10</f>
+        <v>10</v>
+      </c>
+      <c r="L10">
+        <f>J10-'no constraints'!J10</f>
+        <v>2.6357406431206654E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2009</v>
+      </c>
+      <c r="B11">
+        <v>264</v>
+      </c>
+      <c r="C11">
+        <v>164</v>
+      </c>
+      <c r="D11">
+        <v>1352</v>
+      </c>
+      <c r="E11">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>67</v>
+      </c>
+      <c r="G11">
+        <v>7.9998970031738195E-3</v>
+      </c>
+      <c r="H11">
+        <v>4057</v>
+      </c>
+      <c r="I11">
+        <v>3700</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.91200394380083805</v>
+      </c>
+      <c r="K11">
+        <f>I11-'no constraints'!I11</f>
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <f>J11-'no constraints'!J11</f>
+        <v>9.8595020951441903E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12">
+        <v>288</v>
+      </c>
+      <c r="C12">
+        <v>174</v>
+      </c>
+      <c r="D12">
+        <v>1475</v>
+      </c>
+      <c r="E12">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>68</v>
+      </c>
+      <c r="G12">
+        <v>5.9874057769775304E-3</v>
+      </c>
+      <c r="H12">
+        <v>4466</v>
+      </c>
+      <c r="I12">
+        <v>4091</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0.91603224361845048</v>
+      </c>
+      <c r="K12">
+        <f>I12-'no constraints'!I12</f>
+        <v>35</v>
+      </c>
+      <c r="L12">
+        <f>J12-'no constraints'!J12</f>
+        <v>7.8369905956112706E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2011</v>
+      </c>
+      <c r="B13">
+        <v>280</v>
+      </c>
+      <c r="C13">
+        <v>172</v>
+      </c>
+      <c r="D13">
+        <v>1600</v>
+      </c>
+      <c r="E13">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>64</v>
+      </c>
+      <c r="G13">
+        <v>7.9998970031738195E-3</v>
+      </c>
+      <c r="H13">
+        <v>4671</v>
+      </c>
+      <c r="I13">
+        <v>4312</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.92314279597516591</v>
+      </c>
+      <c r="K13">
+        <f>I13-'no constraints'!I13</f>
+        <v>41</v>
+      </c>
+      <c r="L13">
+        <f>J13-'no constraints'!J13</f>
+        <v>8.7775636908584698E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2012</v>
+      </c>
+      <c r="B14">
+        <v>293</v>
+      </c>
+      <c r="C14">
+        <v>175</v>
+      </c>
+      <c r="D14">
+        <v>1659</v>
+      </c>
+      <c r="E14">
+        <v>17</v>
+      </c>
+      <c r="F14">
+        <v>70</v>
+      </c>
+      <c r="G14">
+        <v>8.0018043518066406E-3</v>
+      </c>
+      <c r="H14">
+        <v>4813</v>
+      </c>
+      <c r="I14">
+        <v>4417</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.91772283399127363</v>
+      </c>
+      <c r="K14">
+        <f>I14-'no constraints'!I14</f>
+        <v>17</v>
+      </c>
+      <c r="L14">
+        <f>J14-'no constraints'!J14</f>
+        <v>3.5321005609806333E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2013</v>
+      </c>
+      <c r="B15">
+        <v>320</v>
+      </c>
+      <c r="C15">
+        <v>179</v>
+      </c>
+      <c r="D15">
+        <v>1644</v>
+      </c>
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <v>69</v>
+      </c>
+      <c r="G15">
+        <v>1.2001752853393499E-2</v>
+      </c>
+      <c r="H15">
+        <v>4739</v>
+      </c>
+      <c r="I15">
+        <v>4385</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.92530069634944079</v>
+      </c>
+      <c r="K15">
+        <f>I15-'no constraints'!I15</f>
+        <v>52</v>
+      </c>
+      <c r="L15">
+        <f>J15-'no constraints'!J15</f>
+        <v>1.0972779067313754E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2014</v>
+      </c>
+      <c r="B16">
+        <v>280</v>
+      </c>
+      <c r="C16">
+        <v>183</v>
+      </c>
+      <c r="D16">
+        <v>1635</v>
+      </c>
+      <c r="E16">
+        <v>17</v>
+      </c>
+      <c r="F16">
+        <v>67</v>
+      </c>
+      <c r="G16">
+        <v>6.9813728332519497E-3</v>
+      </c>
+      <c r="H16">
+        <v>4558</v>
+      </c>
+      <c r="I16">
+        <v>4165</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.91377797279508555</v>
+      </c>
+      <c r="K16">
+        <f>I16-'no constraints'!I16</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>J16-'no constraints'!J16</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added level constraint and the tests
</commit_message>
<xml_diff>
--- a/brynmawr/fallAnalysis.xlsx
+++ b/brynmawr/fallAnalysis.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dndin\Documents\CS340\project\cs340-project\brynmawr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E67413-6EC6-4DF5-8D12-D893BA32FAE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADBDD8B-0DEB-4023-801E-16E9781382DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="2475" windowWidth="17040" windowHeight="10800" firstSheet="1" activeTab="4" xr2:uid="{41F0CD19-36E9-4CA9-A6FE-2857FFC324B3}"/>
+    <workbookView xWindow="2130" yWindow="2730" windowWidth="17040" windowHeight="10800" firstSheet="2" activeTab="4" xr2:uid="{41F0CD19-36E9-4CA9-A6FE-2857FFC324B3}"/>
   </bookViews>
   <sheets>
     <sheet name="no constraints" sheetId="1" r:id="rId1"/>
     <sheet name="room constraint" sheetId="2" r:id="rId2"/>
     <sheet name="increasing room size" sheetId="3" r:id="rId3"/>
     <sheet name="limiting subject conflict" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="level constraint" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2998,10 +2998,14 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3060,20 +3064,26 @@
       <c r="F2">
         <v>60</v>
       </c>
+      <c r="G2">
+        <v>1.00095272064208E-2</v>
+      </c>
       <c r="H2">
         <v>3497</v>
       </c>
+      <c r="I2">
+        <v>3140</v>
+      </c>
       <c r="J2">
         <f>I2/H2</f>
-        <v>0</v>
+        <v>0.89791249642550752</v>
       </c>
       <c r="K2">
         <f>I2-'no constraints'!I2</f>
-        <v>-3128</v>
+        <v>12</v>
       </c>
       <c r="L2">
         <f>J2-'no constraints'!J2</f>
-        <v>-0.89448098370031459</v>
+        <v>3.4315127251929312E-3</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3095,20 +3105,26 @@
       <c r="F3">
         <v>59</v>
       </c>
+      <c r="G3">
+        <v>4.0004253387451102E-3</v>
+      </c>
       <c r="H3">
         <v>3542</v>
       </c>
+      <c r="I3">
+        <v>3166</v>
+      </c>
       <c r="J3">
         <f t="shared" ref="J3:J16" si="0">I3/H3</f>
-        <v>0</v>
+        <v>0.89384528514963302</v>
       </c>
       <c r="K3">
         <f>I3-'no constraints'!I3</f>
-        <v>-3173</v>
+        <v>-7</v>
       </c>
       <c r="L3">
         <f>J3-'no constraints'!J3</f>
-        <v>-0.89582156973461324</v>
+        <v>-1.9762845849802257E-3</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3130,20 +3146,26 @@
       <c r="F4">
         <v>61</v>
       </c>
+      <c r="G4">
+        <v>7.9782009124755807E-3</v>
+      </c>
       <c r="H4">
         <v>3579</v>
       </c>
+      <c r="I4">
+        <v>3131</v>
+      </c>
       <c r="J4">
         <f>I4/H4</f>
-        <v>0</v>
+        <v>0.87482537021514395</v>
       </c>
       <c r="K4">
         <f>I4-'no constraints'!I4</f>
-        <v>-3115</v>
+        <v>16</v>
       </c>
       <c r="L4">
         <f>J4-'no constraints'!J4</f>
-        <v>-0.87035484772282756</v>
+        <v>4.4705224923163867E-3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3165,20 +3187,26 @@
       <c r="F5">
         <v>59</v>
       </c>
+      <c r="G5">
+        <v>9.9725723266601493E-3</v>
+      </c>
       <c r="H5">
         <v>3539</v>
       </c>
+      <c r="I5">
+        <v>3149</v>
+      </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.88979937835546763</v>
       </c>
       <c r="K5">
         <f>I5-'no constraints'!I5</f>
-        <v>-3152</v>
+        <v>-3</v>
       </c>
       <c r="L5">
         <f>J5-'no constraints'!J5</f>
-        <v>-0.89064707544504096</v>
+        <v>-8.4769708957332934E-4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3200,20 +3228,26 @@
       <c r="F6">
         <v>51</v>
       </c>
+      <c r="G6">
+        <v>4.8692226409912101E-3</v>
+      </c>
       <c r="H6">
         <v>3700</v>
       </c>
+      <c r="I6">
+        <v>3314</v>
+      </c>
       <c r="J6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.89567567567567563</v>
       </c>
       <c r="K6">
         <f>I6-'no constraints'!I6</f>
-        <v>-3308</v>
+        <v>6</v>
       </c>
       <c r="L6">
         <f>J6-'no constraints'!J6</f>
-        <v>-0.89405405405405403</v>
+        <v>1.6216216216216051E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3235,20 +3269,26 @@
       <c r="F7">
         <v>52</v>
       </c>
+      <c r="G7">
+        <v>3.9987564086914002E-3</v>
+      </c>
       <c r="H7">
         <v>3680</v>
       </c>
+      <c r="I7">
+        <v>3282</v>
+      </c>
       <c r="J7">
         <f>I7/H7</f>
-        <v>0</v>
+        <v>0.89184782608695656</v>
       </c>
       <c r="K7">
         <f>I7-'no constraints'!I7</f>
-        <v>-3266</v>
+        <v>16</v>
       </c>
       <c r="L7">
         <f>J7-'no constraints'!J7</f>
-        <v>-0.88749999999999996</v>
+        <v>4.3478260869566077E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3270,20 +3310,26 @@
       <c r="F8">
         <v>63</v>
       </c>
+      <c r="G8">
+        <v>5.9840679168701102E-3</v>
+      </c>
       <c r="H8">
         <v>3798</v>
       </c>
+      <c r="I8">
+        <v>3393</v>
+      </c>
       <c r="J8">
         <f>I8/H8</f>
-        <v>0</v>
+        <v>0.89336492890995256</v>
       </c>
       <c r="K8">
         <f>I8-'no constraints'!I8</f>
-        <v>-3379</v>
+        <v>14</v>
       </c>
       <c r="L8">
         <f>J8-'no constraints'!J8</f>
-        <v>-0.8896787783043707</v>
+        <v>3.6861506055818616E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3305,20 +3351,26 @@
       <c r="F9">
         <v>62</v>
       </c>
+      <c r="G9">
+        <v>7.9798698425292899E-3</v>
+      </c>
       <c r="H9">
         <v>3862</v>
       </c>
+      <c r="I9">
+        <v>3467</v>
+      </c>
       <c r="J9">
         <f>I9/H9</f>
-        <v>0</v>
+        <v>0.89772138788192646</v>
       </c>
       <c r="K9">
         <f>I9-'no constraints'!I9</f>
-        <v>-3449</v>
+        <v>18</v>
       </c>
       <c r="L9">
         <f>J9-'no constraints'!J9</f>
-        <v>-0.89306059036768515</v>
+        <v>4.6607975142413105E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3340,20 +3392,26 @@
       <c r="F10">
         <v>63</v>
       </c>
+      <c r="G10">
+        <v>1.00271701812744E-2</v>
+      </c>
       <c r="H10">
         <v>3794</v>
       </c>
+      <c r="I10">
+        <v>3403</v>
+      </c>
       <c r="J10">
         <f>I10/H10</f>
-        <v>0</v>
+        <v>0.89694254085397995</v>
       </c>
       <c r="K10">
         <f>I10-'no constraints'!I10</f>
-        <v>-3400</v>
+        <v>3</v>
       </c>
       <c r="L10">
         <f>J10-'no constraints'!J10</f>
-        <v>-0.89615181866104376</v>
+        <v>7.9072219293618851E-4</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3375,20 +3433,26 @@
       <c r="F11">
         <v>67</v>
       </c>
+      <c r="G11">
+        <v>7.9977512359619106E-3</v>
+      </c>
       <c r="H11">
         <v>4057</v>
       </c>
+      <c r="I11">
+        <v>3692</v>
+      </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.91003204338180921</v>
       </c>
       <c r="K11">
         <f>I11-'no constraints'!I11</f>
-        <v>-3660</v>
+        <v>32</v>
       </c>
       <c r="L11">
         <f>J11-'no constraints'!J11</f>
-        <v>-0.90214444170569386</v>
+        <v>7.8876016761153522E-3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3410,20 +3474,26 @@
       <c r="F12">
         <v>68</v>
       </c>
+      <c r="G12">
+        <v>7.0173740386962804E-3</v>
+      </c>
       <c r="H12">
         <v>4466</v>
       </c>
+      <c r="I12">
+        <v>4116</v>
+      </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.92163009404388718</v>
       </c>
       <c r="K12">
         <f>I12-'no constraints'!I12</f>
-        <v>-4056</v>
+        <v>60</v>
       </c>
       <c r="L12">
         <f>J12-'no constraints'!J12</f>
-        <v>-0.90819525302283921</v>
+        <v>1.3434841021047972E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3445,20 +3515,26 @@
       <c r="F13">
         <v>64</v>
       </c>
+      <c r="G13">
+        <v>5.9928894042968698E-3</v>
+      </c>
       <c r="H13">
         <v>4671</v>
       </c>
+      <c r="I13">
+        <v>4287</v>
+      </c>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.91779062299293512</v>
       </c>
       <c r="K13">
         <f>I13-'no constraints'!I13</f>
-        <v>-4271</v>
+        <v>16</v>
       </c>
       <c r="L13">
         <f>J13-'no constraints'!J13</f>
-        <v>-0.91436523228430744</v>
+        <v>3.4253907086276847E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3480,20 +3556,26 @@
       <c r="F14">
         <v>70</v>
       </c>
+      <c r="G14">
+        <v>1.09732151031494E-2</v>
+      </c>
       <c r="H14">
         <v>4813</v>
       </c>
+      <c r="I14">
+        <v>4433</v>
+      </c>
       <c r="J14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.92104716393102015</v>
       </c>
       <c r="K14">
         <f>I14-'no constraints'!I14</f>
-        <v>-4400</v>
+        <v>33</v>
       </c>
       <c r="L14">
         <f>J14-'no constraints'!J14</f>
-        <v>-0.914190733430293</v>
+        <v>6.8564305007271509E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3515,20 +3597,26 @@
       <c r="F15">
         <v>69</v>
       </c>
+      <c r="G15">
+        <v>6.0200691223144497E-3</v>
+      </c>
       <c r="H15">
         <v>4739</v>
       </c>
+      <c r="I15">
+        <v>4341</v>
+      </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.91601603713863688</v>
       </c>
       <c r="K15">
         <f>I15-'no constraints'!I15</f>
-        <v>-4333</v>
+        <v>8</v>
       </c>
       <c r="L15">
         <f>J15-'no constraints'!J15</f>
-        <v>-0.91432791728212703</v>
+        <v>1.688119856509851E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3550,20 +3638,26 @@
       <c r="F16">
         <v>67</v>
       </c>
+      <c r="G16">
+        <v>9.9749565124511701E-3</v>
+      </c>
       <c r="H16">
         <v>4558</v>
       </c>
+      <c r="I16">
+        <v>4173</v>
+      </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.91553312856516011</v>
       </c>
       <c r="K16">
         <f>I16-'no constraints'!I16</f>
-        <v>-4165</v>
+        <v>8</v>
       </c>
       <c r="L16">
         <f>J16-'no constraints'!J16</f>
-        <v>-0.91377797279508555</v>
+        <v>1.7551557700745679E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>